<commit_message>
add classification for op rules, terms, names and facts
</commit_message>
<xml_diff>
--- a/code/outputs/p2_true_pred_results.xlsx
+++ b/code/outputs/p2_true_pred_results.xlsx
@@ -473,16 +473,16 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Any person, including a trustee, who directs or manages the affairs of an unincorporated organization or association other than a partnership.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Any person, including a trustee, who directs or manages, or who participates in directing or managing, the affairs of any unincorporated organization or association other than a partnership.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Any person, including a trustee, who directs or manages, or who participates in directing or managing, the affairs of any unincorporated organization or association other than a partnership.</t>
-        </is>
-      </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0.7473684210526316</v>
       </c>
     </row>
     <row r="3">
@@ -540,7 +540,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Each party named in the process, pleadings, or papers served on the Commission.</t>
+          <t>A party named in the process, pleadings, or papers served.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -561,7 +561,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>An individual, corporation, partnership, or unincorporated organization that resides or has its principal office and place of business in any place not subject to the jurisdiction of the United States.</t>
+          <t>An individual, corporation, partnership, or other unincorporated organization or association that resides in any place not subject to the jurisdiction of the United States.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.4195011337868481</v>
+        <v>0.3809523809523809</v>
       </c>
     </row>
     <row r="7">
@@ -586,7 +586,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Documents served on a non-resident investment adviser, general partner, or managing agent.</t>
+          <t>Legal documents served on a non-resident investment adviser, general partner, or managing agent.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -605,14 +605,10 @@
           <t>Place</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>A location not subject to the jurisdiction of the United States.</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -628,7 +624,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>An individual or entity involved in serving process, pleadings, or papers.</t>
+          <t>Any individual, corporation, partnership, or other unincorporated organization or association.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -649,7 +645,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>An association that has its principal office and place of business in any place not subject to the jurisdiction of the United States.</t>
+          <t>An unincorporated organization or association other than a partnership.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -691,7 +687,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>The records maintained by the Commission where an additional copy of the process, pleadings, or papers is kept.</t>
+          <t>The records maintained by the Commission, which include a copy of the process, pleadings, or papers served.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -712,7 +708,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>The Secretary of the Commission (Secretary) will promptly forward a copy to each named party by registered or certified mail at that party's last address filed with the Commission.</t>
+          <t>The Secretary of the Commission is responsible for forwarding a copy of the process, pleadings, or papers to each named party by registered or certified mail.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -733,7 +729,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>The section where a person may serve a non-resident investment adviser, general partner, or managing agent by furnishing the Commission with copies of the documents.</t>
+          <t>A section of the document describing the service of process, pleadings, or papers on the Commission.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -754,7 +750,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>The main office of a corporation, partnership, or unincorporated organization.</t>
+          <t>The main office and place of business, as defined in § 275.203A-3(c) of this chapter.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -775,7 +771,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>The section that defines 'Principal office and place of business'.</t>
+          <t>A section of the chapter that defines 'Principal office and place of business.'</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -794,14 +790,10 @@
           <t>Evidence of service</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Certification by the Secretary that the Commission was served with documents and forwarded them to a named party.</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -817,7 +809,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>A person who directs or manages the affairs of any unincorporated organization or association other than a partnership.</t>
+          <t>A person who directs or manages the affairs of an unincorporated organization or association.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -838,7 +830,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>A corporation that is incorporated in or that has its principal office and place of business in any place not subject to the jurisdiction of the United States.</t>
+          <t>A corporation that is incorporated in or has its principal office and place of business in any place not subject to the jurisdiction of the United States.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -859,7 +851,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>An organization that is not incorporated and has its principal office and place of business in any place not subject to the jurisdiction of the United States.</t>
+          <t>An organization or association that is not incorporated and is managed by a managing agent.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -880,7 +872,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>A method used by the Secretary to forward documents to named parties.</t>
+          <t>A method of mailing used by the Secretary to forward a copy of the process, pleadings, or papers to each named party.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -922,7 +914,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>The act of the Secretary certifying that the Commission was served with documents and forwarded them to a named party.</t>
+          <t>The Secretary's certification that the Commission was served with process, pleadings, or other papers and forwarded these documents to a named party.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
@@ -943,7 +935,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>The section where the Secretary of the Commission forwards a copy to each named party by registered or certified mail.</t>
+          <t>A section of the document describing the forwarding of documents by the Secretary to a named party by registered or certified mail.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -964,7 +956,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>The location where a corporation, partnership, or unincorporated organization conducts its business.</t>
+          <t>The location where the main business activities are conducted, as defined in § 275.203A-3(c) of this chapter.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -983,14 +975,10 @@
           <t>Jurisdiction of the United States</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>The legal authority or control of the United States over a place.</t>
-        </is>
-      </c>
+      <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1006,7 +994,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Activities directed or managed by a managing agent of any unincorporated organization or association other than a partnership.</t>
+          <t>The activities directed or managed by a managing agent of an unincorporated organization or association.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -1027,7 +1015,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Agents appointed to receive service of process, pleadings, or papers on behalf of a non-resident investment adviser, general partner, or managing agent.</t>
+          <t>Agents appointed to receive service of process, pleadings, or other papers on behalf of a non-resident investment adviser, general partner, or managing agent.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -1069,7 +1057,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Legal documents served on a non-resident investment adviser, general partner, or managing agent.</t>
+          <t>The legal documents served on a non-resident investment adviser, general partner, or managing agent.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -1088,14 +1076,10 @@
           <t>Papers</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Documents served on a non-resident investment adviser, general partner, or managing agent.</t>
-        </is>
-      </c>
+      <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1111,7 +1095,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>The Secretary of the Commission who forwards documents to named parties.</t>
+          <t>The Secretary of the Commission responsible for forwarding documents to named parties.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -1130,14 +1114,10 @@
           <t>Investment adviser</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>An adviser who provides investment advice and may be served with process, pleadings, or papers.</t>
-        </is>
-      </c>
+      <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1153,7 +1133,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>The last address filed with the Commission by a named party.</t>
+          <t>The last address filed with the Commission for a named party.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -1174,7 +1154,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>A method used by the Secretary to forward documents to named parties.</t>
+          <t>A method of mailing used by the Secretary to forward a copy of the process, pleadings, or papers to each named party.</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -1195,7 +1175,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>The entity to which a person may furnish copies of process, pleadings, or papers for service on non-resident investment advisers, general partners, or managing agents.</t>
+          <t>The entity responsible for receiving service of process, pleadings, or other papers on behalf of non-resident investment advisers, general partners, or managing agents.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -1241,7 +1221,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Reasons for requesting a hearing must be stated by the interested person.</t>
+          <t>Interested persons must state their reasons for requesting a hearing.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1250,7 +1230,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.1857585139318886</v>
+        <v>0.1888544891640866</v>
       </c>
     </row>
     <row r="39">
@@ -1266,7 +1246,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Refers to the Act under which the Commission operates and makes orders.</t>
+          <t>Any section of the Act or any rule or regulation thereunder.</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1275,7 +1255,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.25</v>
+        <v>0.8194444444444444</v>
       </c>
     </row>
     <row r="40">
@@ -1291,16 +1271,16 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t>An application for registration as an investment adviser is excluded from the definition of 'application'.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
           <t>An application for registration as an investment adviser.</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>An application for registration as an investment adviser.</t>
-        </is>
-      </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>0.5377358490566038</v>
       </c>
     </row>
     <row r="41">
@@ -1341,7 +1321,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>An interested person may submit facts and request a hearing, stating reasons and the nature of their interest.</t>
+          <t>Any person who may submit facts and request a hearing on the matter.</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1350,7 +1330,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.3504672897196262</v>
+        <v>0.2897196261682243</v>
       </c>
     </row>
     <row r="43">
@@ -1391,7 +1371,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>The publication where notice of the initiation of the proceeding will be published.</t>
+          <t>Notice of the initiation of the proceeding will be published in the Federal Register.</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1400,7 +1380,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.4470588235294117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1466,7 +1446,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>A hearing may be ordered if necessary or appropriate in the public interest or for the protection of investors.</t>
+          <t>May be ordered if necessary or appropriate in the public interest or for the protection of investors.</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1475,7 +1455,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.6144578313253012</v>
+        <v>0.572289156626506</v>
       </c>
     </row>
     <row r="48">
@@ -1491,7 +1471,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>A factor considered by the Commission to determine the necessity of a hearing.</t>
+          <t>A hearing may be ordered if necessary or appropriate in the public interest.</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1500,7 +1480,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.3053435114503816</v>
+        <v>0.5114503816793894</v>
       </c>
     </row>
     <row r="49">
@@ -1541,7 +1521,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Facts bearing upon the desirability of a hearing on the matter may be submitted by an interested person.</t>
+          <t>Interested persons may submit facts bearing upon the desirability of a hearing.</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1550,7 +1530,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.2742857142857142</v>
+        <v>0.4342857142857143</v>
       </c>
     </row>
     <row r="51">
@@ -1591,7 +1571,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>An application means any application for an order of the Commission under the Act other than an application for registration as an investment adviser.</t>
+          <t>An 'application' means any application for an order of the Commission under the Act other than an application for registration as an investment adviser.</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1641,7 +1621,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>The specified duration within which actions must be taken or submissions made.</t>
+          <t>The period within which interested persons may submit facts and request a hearing.</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1650,7 +1630,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>0.2514285714285714</v>
+        <v>0.3257142857142857</v>
       </c>
     </row>
     <row r="55">
@@ -1666,7 +1646,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>The body that initiates proceedings, issues orders, and may order hearings.</t>
+          <t>The body that may initiate proceedings and order hearings.</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1675,7 +1655,7 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>0.2710843373493976</v>
+        <v>0.2469879518072289</v>
       </c>
     </row>
     <row r="56">
@@ -1716,7 +1696,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>The subject of the proceeding initiated by the application or Commission's motion.</t>
+          <t>The subject of the proceeding or hearing.</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1725,7 +1705,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>0.2810457516339869</v>
+        <v>0.2026143790849673</v>
       </c>
     </row>
     <row r="58">
@@ -1739,14 +1719,18 @@
           <t>Managing agent</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>A person is presumed to control a trust if the person is a trustee or managing agent of the trust.</t>
+        </is>
+      </c>
       <c r="D58" t="inlineStr">
         <is>
           <t>A person is presumed to control a trust if the person is a trustee or managing agent of the trust.</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -1762,16 +1746,16 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
+          <t>A small business or small organization for purposes of the Investment Advisers Act of 1940 is an investment adviser with assets under management of less than $25 million, did not have total assets of $5 million or more on the last day of the most recent fiscal year, and does not control, is not controlled by, and is not under common control with another investment adviser with assets under management of $25 million or more.</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
           <t>An investment adviser that has assets under management of less than $25 million, did not have total assets of $5 million or more on the last day of the most recent fiscal year, and does not control, is not controlled by, and is not under common control with another investment adviser that has assets under management of $25 million or more, or any person (other than a natural person) that had total assets of $5 million or more on the last day of the most recent fiscal year.</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>An investment adviser that has assets under management of less than $25 million, did not have total assets of $5 million or more on the last day of the most recent fiscal year, and does not control, is not controlled by, and is not under common control with another investment adviser that has assets under management of $25 million or more, or any person (other than a natural person) that had total assets of $5 million or more on the last day of the most recent fiscal year.</t>
-        </is>
-      </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>0.5052410901467506</v>
       </c>
     </row>
     <row r="60">
@@ -1785,14 +1769,18 @@
           <t>Partnership</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>A person is presumed to control a partnership if the person has the right to receive upon dissolution, or has contributed, 25 percent or more of the capital of the partnership.</t>
+        </is>
+      </c>
       <c r="D60" t="inlineStr">
         <is>
           <t>A person is presumed to control a partnership if the person has the right to receive upon dissolution, or has contributed, 25 percent or more of the capital of the partnership.</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1806,10 +1794,14 @@
           <t>Investment Advisers Act of 1940</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>The Investment Advisers Act of 1940 is referenced in defining a small business or small organization as an investment adviser with certain asset criteria.</t>
+        </is>
+      </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1857,14 +1849,18 @@
           <t>Trust</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>A person is presumed to control a trust if the person is a trustee or managing agent of the trust.</t>
+        </is>
+      </c>
       <c r="D64" t="inlineStr">
         <is>
           <t>A person is presumed to control a trust if the person is a trustee or managing agent of the trust.</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -1878,14 +1874,18 @@
           <t>Person</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>A person is presumed to control a corporation, partnership, LLC, or trust under certain conditions outlined in the document.</t>
+        </is>
+      </c>
       <c r="D65" t="inlineStr">
         <is>
           <t>A person is presumed to control a corporation if the person directly or indirectly has the right to vote 25 percent or more of a class of the corporation's voting securities or has the power to sell or direct the sale of 25 percent or more of a class of the corporation's voting securities.</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>0.3241379310344827</v>
       </c>
     </row>
     <row r="66">
@@ -1916,10 +1916,14 @@
           <t>Class of the interests</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr"/>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>A person is presumed to control an LLC if the person has the right to vote 25 percent or more of a class of the interests of the LLC.</t>
+        </is>
+      </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1933,14 +1937,18 @@
           <t>Right to receive upon dissolution</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>A person is presumed to control a partnership if the person has the right to receive upon dissolution, or has contributed, 25 percent or more of the capital of the partnership.</t>
+        </is>
+      </c>
       <c r="D68" t="inlineStr">
         <is>
           <t>A person is presumed to control a partnership if the person has the right to receive upon dissolution, or has contributed, 25 percent or more of the capital of the partnership.</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -1956,7 +1964,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Assets under management, as defined under Section 203A(a)(3) of the Act and reported on its annual updating amendment to Form ADV, of less than $25 million, or such higher amount as the Commission may by rule deem appropriate.</t>
+          <t>Assets under management are defined under Section 203A(a)(3) of the Act and reported on the annual updating amendment to Form ADV.</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1965,7 +1973,7 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>0.8528301886792453</v>
+        <v>0.4679245283018868</v>
       </c>
     </row>
     <row r="70">
@@ -2025,14 +2033,18 @@
           <t>Balance sheet</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr"/>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Total assets means the total assets as shown on the balance sheet of the investment adviser or other person, or the balance sheet of the investment adviser or such other person with its subsidiaries consolidated, whichever is larger.</t>
+        </is>
+      </c>
       <c r="D72" t="inlineStr">
         <is>
           <t>The total assets as shown on the balance sheet of the investment adviser or other person described, or the balance sheet of the investment adviser or such other person with its subsidiaries consolidated, whichever is larger.</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>0.8755364806866953</v>
       </c>
     </row>
     <row r="73">
@@ -2048,7 +2060,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>The total assets as shown on the balance sheet of the investment adviser or other person, or the balance sheet of the investment adviser or such other person with its subsidiaries consolidated, whichever is larger.</t>
+          <t>Total assets means the total assets as shown on the balance sheet of the investment adviser or other person, or the balance sheet of the investment adviser or such other person with its subsidiaries consolidated, whichever is larger.</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2057,7 +2069,7 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0.9363636363636364</v>
+        <v>0.8583690987124464</v>
       </c>
     </row>
     <row r="74">
@@ -2073,16 +2085,16 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
+          <t>A small business or small organization for purposes of the Investment Advisers Act of 1940 is an investment adviser with assets under management of less than $25 million, did not have total assets of $5 million or more on the last day of the most recent fiscal year, and does not control, is not controlled by, and is not under common control with another investment adviser with assets under management of $25 million or more.</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
           <t>An investment adviser that has assets under management of less than $25 million, did not have total assets of $5 million or more on the last day of the most recent fiscal year, and does not control, is not controlled by, and is not under common control with another investment adviser that has assets under management of $25 million or more, or any person (other than a natural person) that had total assets of $5 million or more on the last day of the most recent fiscal year.</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>An investment adviser that has assets under management of less than $25 million, did not have total assets of $5 million or more on the last day of the most recent fiscal year, and does not control, is not controlled by, and is not under common control with another investment adviser that has assets under management of $25 million or more, or any person (other than a natural person) that had total assets of $5 million or more on the last day of the most recent fiscal year.</t>
-        </is>
-      </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>0.5052410901467506</v>
       </c>
     </row>
     <row r="75">
@@ -2096,14 +2108,18 @@
           <t>Trustee</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr"/>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>A person is presumed to control a trust if the person is a trustee or managing agent of the trust.</t>
+        </is>
+      </c>
       <c r="D75" t="inlineStr">
         <is>
           <t>A person is presumed to control a trust if the person is a trustee or managing agent of the trust.</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -2117,14 +2133,18 @@
           <t>Corporation</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>A person is presumed to control a corporation if the person directly or indirectly has the right to vote 25 percent or more of a class of the corporation's voting securities, or has the power to sell or direct the sale of 25 percent or more of a class of the corporation's voting securities.</t>
+        </is>
+      </c>
       <c r="D76" t="inlineStr">
         <is>
           <t>A person is presumed to control a corporation if the person directly or indirectly has the right to vote 25 percent or more of a class of the corporation's voting securities or has the power to sell or direct the sale of 25 percent or more of a class of the corporation's voting securities.</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>0.9965635738831615</v>
       </c>
     </row>
     <row r="77">
@@ -2140,7 +2160,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>An investment adviser that has assets under management of less than $25 million, or such higher amount as the Commission may by rule deem appropriate, did not have total assets of $5 million or more on the last day of the most recent fiscal year, and does not control, is not controlled by, and is not under common control with another investment adviser that has assets under management of $25 million or more, or any person (other than a natural person) that had total assets of $5 million or more on the last day of the most recent fiscal year.</t>
+          <t>An investment adviser is a small business or small organization under the Investment Advisers Act of 1940 if it has assets under management of less than $25 million, did not have total assets of $5 million or more on the last day of the most recent fiscal year, and does not control, is not controlled by, and is not under common control with another investment adviser with assets under management of $25 million or more.</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2149,7 +2169,7 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>0.8720292504570384</v>
+        <v>0.5220125786163522</v>
       </c>
     </row>
     <row r="78">
@@ -2163,14 +2183,18 @@
           <t>Capital of the partnership</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr"/>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>A person is presumed to control a partnership if the person has the right to receive upon dissolution, or has contributed, 25 percent or more of the capital of the partnership.</t>
+        </is>
+      </c>
       <c r="D78" t="inlineStr">
         <is>
           <t>A person is presumed to control a partnership if the person has the right to receive upon dissolution, or has contributed, 25 percent or more of the capital of the partnership.</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -2186,16 +2210,16 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
+          <t>A person is presumed to control a corporation if the person has the right to vote 25 percent or more of a class of the corporation's voting securities.</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
           <t>A person is presumed to control a corporation if the person directly or indirectly has the right to vote 25 percent or more of a class of the corporation's voting securities or has the power to sell or direct the sale of 25 percent or more of a class of the corporation's voting securities.</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>A person is presumed to control a corporation if the person directly or indirectly has the right to vote 25 percent or more of a class of the corporation's voting securities or has the power to sell or direct the sale of 25 percent or more of a class of the corporation's voting securities.</t>
-        </is>
-      </c>
       <c r="E79" t="n">
-        <v>1</v>
+        <v>0.5206896551724138</v>
       </c>
     </row>
     <row r="80">
@@ -2211,16 +2235,16 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
+          <t>Control means the power, directly or indirectly, to direct the management or policies of a person, whether through ownership of securities, by contract, or otherwise.</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
           <t>The power, directly or indirectly, to direct the management or policies of a person, whether through ownership of securities, by contract, or otherwise.</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>The power, directly or indirectly, to direct the management or policies of a person, whether through ownership of securities, by contract, or otherwise.</t>
-        </is>
-      </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>0.9096385542168675</v>
       </c>
     </row>
     <row r="81">
@@ -2251,14 +2275,18 @@
           <t>Right to vote</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr"/>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>A person is presumed to control a corporation if the person directly or indirectly has the right to vote 25 percent or more of a class of the corporation's voting securities.</t>
+        </is>
+      </c>
       <c r="D82" t="inlineStr">
         <is>
           <t>A person is presumed to control a corporation if the person directly or indirectly has the right to vote 25 percent or more of a class of the corporation's voting securities.</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">

</xml_diff>